<commit_message>
updated thoughts and visualization
</commit_message>
<xml_diff>
--- a/creditorsGraphed.xlsx
+++ b/creditorsGraphed.xlsx
@@ -197,10 +197,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="134"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="34"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2709,35 +2709,6 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3070,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new graphs with percentages
</commit_message>
<xml_diff>
--- a/creditorsGraphed.xlsx
+++ b/creditorsGraphed.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="OverallSort" sheetId="1" r:id="rId1"/>
+    <sheet name="PercentageSorting" sheetId="2" r:id="rId2"/>
+    <sheet name="PercentageSortingShort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
   <si>
     <t>Cesnola Collection</t>
   </si>
@@ -145,7 +145,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,14 +182,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -216,7 +232,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>OverallSort!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -228,7 +244,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -278,7 +294,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$O$2</c:f>
+              <c:f>OverallSort!$B$2:$O$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -333,7 +349,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>OverallSort!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -345,7 +361,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -395,7 +411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$O$3</c:f>
+              <c:f>OverallSort!$B$3:$O$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -450,7 +466,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>OverallSort!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -462,7 +478,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -512,7 +528,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$O$4</c:f>
+              <c:f>OverallSort!$B$4:$O$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -567,7 +583,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>OverallSort!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -579,7 +595,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -629,7 +645,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$O$5</c:f>
+              <c:f>OverallSort!$B$5:$O$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -684,7 +700,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>OverallSort!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -696,7 +712,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -746,7 +762,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$O$6</c:f>
+              <c:f>OverallSort!$B$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -801,7 +817,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>OverallSort!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -813,7 +829,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -863,7 +879,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$O$7</c:f>
+              <c:f>OverallSort!$B$7:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -918,7 +934,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>OverallSort!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -930,7 +946,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -980,7 +996,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$O$8</c:f>
+              <c:f>OverallSort!$B$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1035,7 +1051,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>OverallSort!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1047,7 +1063,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1097,7 +1113,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$O$9</c:f>
+              <c:f>OverallSort!$B$9:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1152,7 +1168,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>OverallSort!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1164,7 +1180,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1214,7 +1230,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$O$10</c:f>
+              <c:f>OverallSort!$B$10:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1269,7 +1285,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>OverallSort!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1281,7 +1297,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1331,7 +1347,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$O$11</c:f>
+              <c:f>OverallSort!$B$11:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1386,7 +1402,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>OverallSort!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1398,7 +1414,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1448,7 +1464,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$O$12</c:f>
+              <c:f>OverallSort!$B$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1503,7 +1519,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>OverallSort!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1515,7 +1531,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1565,7 +1581,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$O$13</c:f>
+              <c:f>OverallSort!$B$13:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1620,7 +1636,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>OverallSort!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1632,7 +1648,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1682,7 +1698,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$O$14</c:f>
+              <c:f>OverallSort!$B$14:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1737,7 +1753,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>OverallSort!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1749,7 +1765,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1799,7 +1815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$O$15</c:f>
+              <c:f>OverallSort!$B$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1854,7 +1870,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>OverallSort!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1866,7 +1882,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1916,7 +1932,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$O$16</c:f>
+              <c:f>OverallSort!$B$16:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1971,7 +1987,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>OverallSort!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1983,7 +1999,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2033,7 +2049,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$O$17</c:f>
+              <c:f>OverallSort!$B$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2088,7 +2104,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$18</c:f>
+              <c:f>OverallSort!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2100,7 +2116,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2150,7 +2166,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$O$18</c:f>
+              <c:f>OverallSort!$B$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2205,7 +2221,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$19</c:f>
+              <c:f>OverallSort!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2217,7 +2233,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2267,7 +2283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$O$19</c:f>
+              <c:f>OverallSort!$B$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2322,7 +2338,7 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$20</c:f>
+              <c:f>OverallSort!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2334,7 +2350,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2384,7 +2400,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$O$20</c:f>
+              <c:f>OverallSort!$B$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2439,7 +2455,7 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
+              <c:f>OverallSort!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2451,7 +2467,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2501,7 +2517,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$O$21</c:f>
+              <c:f>OverallSort!$B$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2556,7 +2572,7 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$22</c:f>
+              <c:f>OverallSort!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2568,7 +2584,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2618,7 +2634,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$22:$O$22</c:f>
+              <c:f>OverallSort!$B$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2673,7 +2689,7 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$23</c:f>
+              <c:f>OverallSort!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2685,7 +2701,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2735,7 +2751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$O$23</c:f>
+              <c:f>OverallSort!$B$23:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2790,7 +2806,7 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$24</c:f>
+              <c:f>OverallSort!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2802,7 +2818,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2852,7 +2868,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$O$24</c:f>
+              <c:f>OverallSort!$B$24:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2907,7 +2923,7 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$25</c:f>
+              <c:f>OverallSort!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2919,7 +2935,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2969,7 +2985,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$25:$O$25</c:f>
+              <c:f>OverallSort!$B$25:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -3024,7 +3040,7 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$26</c:f>
+              <c:f>OverallSort!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3036,7 +3052,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -3086,7 +3102,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$O$26</c:f>
+              <c:f>OverallSort!$B$26:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -3141,7 +3157,7 @@
           <c:order val="25"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$27</c:f>
+              <c:f>OverallSort!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3153,7 +3169,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$O$1</c:f>
+              <c:f>OverallSort!$B$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -3203,7 +3219,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$O$27</c:f>
+              <c:f>OverallSort!$B$27:$O$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -3263,20 +3279,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="101743104"/>
-        <c:axId val="84460672"/>
+        <c:axId val="117099520"/>
+        <c:axId val="87598208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101743104"/>
+        <c:axId val="117099520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84460672"/>
+        <c:crossAx val="87598208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3284,7 +3301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84460672"/>
+        <c:axId val="87598208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3295,7 +3312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101743104"/>
+        <c:crossAx val="117099520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3304,6 +3321,241 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PercentageSorting!$A$1:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>vases</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>glass</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gold and silver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>terracotta</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>bronze</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gem</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>stone</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lead</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>coins</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>otherObjects</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>bone</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>amber</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>paintings</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Faience</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>iron</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>clay</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>mosaic</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>stucco</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>shell</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>plaster</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>forgery</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>documents</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>wood</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>book</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>papyrus</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>wax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PercentageSorting!$Q$1:$Q$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.29933169187478015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15617305663032008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11419861648493375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1026497830929769</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10165318325712276</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.373900809004572E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.2986282096377073E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2135068589518115E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8521514831750494E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7935279634189234E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.3831633251260397E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.9727986868331577E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9277758236604529E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.2242935865869388E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5828350334154062E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5828350334154062E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0552233556102709E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4485871731738778E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9311759878063078E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3449407902450463E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7587055926837847E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1724703951225231E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1724703951225231E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.8623519756126157E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.8623519756126157E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8623519756126157E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3338,6 +3590,41 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noChangeAspect="1"/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3641,10 +3928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,10 +3950,11 @@
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3710,7 +3998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3760,8 +4048,9 @@
         <f>SUM(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2)</f>
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3808,11 +4097,12 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P28" si="0">SUM(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3)</f>
+        <f>SUM(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3859,11 +4149,12 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f>SUM(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4,O4)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3913,8 +4204,9 @@
         <f>SUM(B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5,M5,N5,O5)</f>
         <v>1734</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3961,11 +4253,12 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
+        <f>SUM(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6)</f>
         <v>1599</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4012,11 +4305,12 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
+        <f>SUM(B7,C7,D7,E7,F7,G7,H7,I7,J7,K7,L7,M7,N7,O7)</f>
         <v>2664</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4063,11 +4357,12 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f>SUM(B8,C8,D8,E8,F8,G8,H8,I8,J8,K8,L8,M8,N8,O8)</f>
         <v>1948</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4114,11 +4409,12 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
+        <f>SUM(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9)</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4165,11 +4461,12 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f>SUM(B10,C10,D10,E10,F10,G10,H10,I10,J10,K10,L10,M10,N10,O10)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4216,11 +4513,12 @@
         <v>180</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
+        <f>SUM(B11,C11,D11,E11,F11,G11,H11,I11,J11,K11,L11,M11,N11,O11)</f>
         <v>207</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4267,11 +4565,12 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
+        <f>SUM(B12,C12,D12,E12,F12,G12,H12,I12,J12,K12,L12,M12,N12,O12)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4318,11 +4617,12 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="0"/>
+        <f>SUM(B13,C13,D13,E13,F13,G13,H13,I13,J13,K13,L13,M13,N13,O13)</f>
         <v>1245</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -4369,11 +4669,12 @@
         <v>3</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f>SUM(B14,C14,D14,E14,F14,G14,H14,I14,J14,K14,L14,M14,N14,O14)</f>
         <v>1751</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -4420,11 +4721,12 @@
         <v>51</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f>SUM(B15,C15,D15,E15,F15,G15,H15,I15,J15,K15,L15,M15,N15,O15)</f>
         <v>5106</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4471,11 +4773,12 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f>SUM(B16,C16,D16,E16,F16,G16,H16,I16,J16,K16,L16,M16,N16,O16)</f>
         <v>136</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -4522,11 +4825,12 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f>SUM(B17,C17,D17,E17,F17,G17,H17,I17,J17,K17,L17,M17,N17,O17)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -4573,11 +4877,12 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
+        <f>SUM(B18,C18,D18,E18,F18,G18,H18,I18,J18,K18,L18,M18,N18,O18)</f>
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -4624,11 +4929,12 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
+        <f>SUM(B19,C19,D19,E19,F19,G19,H19,I19,J19,K19,L19,M19,N19,O19)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -4675,11 +4981,12 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
+        <f>SUM(B20,C20,D20,E20,F20,G20,H20,I20,J20,K20,L20,M20,N20,O20)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -4726,11 +5033,12 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <f t="shared" si="0"/>
+        <f>SUM(B21,C21,D21,E21,F21,G21,H21,I21,J21,K21,L21,M21,N21,O21)</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -4777,11 +5085,12 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" si="0"/>
+        <f>SUM(B22,C22,D22,E22,F22,G22,H22,I22,J22,K22,L22,M22,N22,O22)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -4828,11 +5137,12 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <f t="shared" si="0"/>
+        <f>SUM(B23,C23,D23,E23,F23,G23,H23,I23,J23,K23,L23,M23,N23,O23)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -4879,11 +5189,12 @@
         <v>0</v>
       </c>
       <c r="P24">
-        <f t="shared" si="0"/>
+        <f>SUM(B24,C24,D24,E24,F24,G24,H24,I24,J24,K24,L24,M24,N24,O24)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -4930,11 +5241,12 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f>SUM(B25,C25,D25,E25,F25,G25,H25,I25,J25,K25,L25,M25,N25,O25)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -4981,11 +5293,12 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f>SUM(B26,C26,D26,E26,F26,G26,H26,I26,J26,K26,L26,M26,N26,O26)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -4998,59 +5311,60 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:O27" si="1">SUM(D28,-D2,-D3,-D4,-D5,-D6,-D7,-D8,-D9,-D10,-D11,-D12,-D13,-D14,-D15,-D16,-D17,-D18,-D19,-D20,-D21,-D22,-D23,-D24,-D25,-D26)</f>
+        <f>SUM(D28,-D2,-D3,-D4,-D5,-D6,-D7,-D8,-D9,-D10,-D11,-D12,-D13,-D14,-D15,-D16,-D17,-D18,-D19,-D20,-D21,-D22,-D23,-D24,-D25,-D26)</f>
         <v>36</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f>SUM(E28,-E2,-E3,-E4,-E5,-E6,-E7,-E8,-E9,-E10,-E11,-E12,-E13,-E14,-E15,-E16,-E17,-E18,-E19,-E20,-E21,-E22,-E23,-E24,-E25,-E26)</f>
         <v>3</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f>SUM(F28,-F2,-F3,-F4,-F5,-F6,-F7,-F8,-F9,-F10,-F11,-F12,-F13,-F14,-F15,-F16,-F17,-F18,-F19,-F20,-F21,-F22,-F23,-F24,-F25,-F26)</f>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f>SUM(G28,-G2,-G3,-G4,-G5,-G6,-G7,-G8,-G9,-G10,-G11,-G12,-G13,-G14,-G15,-G16,-G17,-G18,-G19,-G20,-G21,-G22,-G23,-G24,-G25,-G26)</f>
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f>SUM(H28,-H2,-H3,-H4,-H5,-H6,-H7,-H8,-H9,-H10,-H11,-H12,-H13,-H14,-H15,-H16,-H17,-H18,-H19,-H20,-H21,-H22,-H23,-H24,-H25,-H26)</f>
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f>SUM(I28,-I2,-I3,-I4,-I5,-I6,-I7,-I8,-I9,-I10,-I11,-I12,-I13,-I14,-I15,-I16,-I17,-I18,-I19,-I20,-I21,-I22,-I23,-I24,-I25,-I26)</f>
         <v>1</v>
       </c>
       <c r="J27">
-        <f t="shared" si="1"/>
+        <f>SUM(J28,-J2,-J3,-J4,-J5,-J6,-J7,-J8,-J9,-J10,-J11,-J12,-J13,-J14,-J15,-J16,-J17,-J18,-J19,-J20,-J21,-J22,-J23,-J24,-J25,-J26)</f>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f>SUM(K28,-K2,-K3,-K4,-K5,-K6,-K7,-K8,-K9,-K10,-K11,-K12,-K13,-K14,-K15,-K16,-K17,-K18,-K19,-K20,-K21,-K22,-K23,-K24,-K25,-K26)</f>
         <v>2</v>
       </c>
       <c r="L27">
-        <f t="shared" si="1"/>
+        <f>SUM(L28,-L2,-L3,-L4,-L5,-L6,-L7,-L8,-L9,-L10,-L11,-L12,-L13,-L14,-L15,-L16,-L17,-L18,-L19,-L20,-L21,-L22,-L23,-L24,-L25,-L26)</f>
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="1"/>
+        <f>SUM(M28,-M2,-M3,-M4,-M5,-M6,-M7,-M8,-M9,-M10,-M11,-M12,-M13,-M14,-M15,-M16,-M17,-M18,-M19,-M20,-M21,-M22,-M23,-M24,-M25,-M26)</f>
         <v>1</v>
       </c>
       <c r="N27">
-        <f t="shared" si="1"/>
+        <f>SUM(N28,-N2,-N3,-N4,-N5,-N6,-N7,-N8,-N9,-N10,-N11,-N12,-N13,-N14,-N15,-N16,-N17,-N18,-N19,-N20,-N21,-N22,-N23,-N24,-N25,-N26)</f>
         <v>0</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
+        <f>SUM(O28,-O2,-O3,-O4,-O5,-O6,-O7,-O8,-O9,-O10,-O11,-O12,-O13,-O14,-O15,-O16,-O17,-O18,-O19,-O20,-O21,-O22,-O23,-O24,-O25,-O26)</f>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f>SUM(B27,C27,D27,E27,F27,G27,H27,I27,J27,K27,L27,M27,N27,O27)</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -5097,36 +5411,1639 @@
         <v>239</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f>SUM(B28,C28,D28,E28,F28,G28,H28,I28,J28,K28,L28,M28,N28,O28)</f>
         <v>17058</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>1215</v>
+      </c>
+      <c r="C1">
+        <v>1224</v>
+      </c>
+      <c r="D1">
+        <v>1024</v>
+      </c>
+      <c r="E1">
+        <v>457</v>
+      </c>
+      <c r="F1">
+        <v>392</v>
+      </c>
+      <c r="G1">
+        <v>26</v>
+      </c>
+      <c r="H1">
+        <v>224</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>22</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>244</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>227</v>
+      </c>
+      <c r="O1">
+        <v>51</v>
+      </c>
+      <c r="P1">
+        <v>5106</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>0.29933169187478015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>495</v>
+      </c>
+      <c r="C2">
+        <v>57</v>
+      </c>
+      <c r="D2">
+        <v>290</v>
+      </c>
+      <c r="E2">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>822</v>
+      </c>
+      <c r="G2">
+        <v>612</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>333</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>2664</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.15617305663032008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>1285</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <v>155</v>
+      </c>
+      <c r="E3">
+        <v>303</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1948</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.11419861648493375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>845</v>
+      </c>
+      <c r="C4">
+        <v>399</v>
+      </c>
+      <c r="D4">
+        <v>229</v>
+      </c>
+      <c r="E4">
+        <v>71</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>77</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>76</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>1751</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.1026497830929769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>449</v>
+      </c>
+      <c r="C5">
+        <v>470</v>
+      </c>
+      <c r="D5">
+        <v>297</v>
+      </c>
+      <c r="E5">
+        <v>298</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>115</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>36</v>
+      </c>
+      <c r="K5">
+        <v>22</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>13</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1734</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.10165318325712276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>129</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>120</v>
+      </c>
+      <c r="E6">
+        <v>85</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>497</v>
+      </c>
+      <c r="J6">
+        <v>338</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>281</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1599</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>9.373900809004572E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>593</v>
+      </c>
+      <c r="C7">
+        <v>245</v>
+      </c>
+      <c r="D7">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>39</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1245</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>7.2986282096377073E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>180</v>
+      </c>
+      <c r="P8">
+        <v>207</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.2135068589518115E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>46</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>151</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>8.8521514831750494E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>150</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>8.7935279634189234E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>143</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>8.3831633251260397E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>105</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>136</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>7.9727986868331577E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>3.9277758236604529E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>55</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>3.2242935865869388E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.5828350334154062E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1.5828350334154062E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1.0552233556102709E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>6.4485871731738778E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>2.9311759878063078E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2.3449407902450463E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1.7587055926837847E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1.1724703951225231E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1.1724703951225231E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:Q26">
+    <sortCondition descending="1" ref="Q1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.29933169187478015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.15617305663032008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.11419861648493375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.1026497830929769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.10165318325712276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9.373900809004572E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7.2986282096377073E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.2135068589518115E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8.8521514831750494E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8.7935279634189234E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8.3831633251260397E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7.9727986868331577E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.9277758236604529E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.2242935865869388E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.5828350334154062E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.5828350334154062E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.0552233556102709E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2">
+        <v>6.4485871731738778E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2.9311759878063078E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.3449407902450463E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.7587055926837847E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.1724703951225231E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.1724703951225231E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5.8623519756126157E-5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>